<commit_message>
Modifs schéma & réorganisation
Modifs schéma & réorganisation JS
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js859\Desktop\OC\P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B383277C-034E-4038-B495-AC2DB9F97617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0DB23-1A01-4014-9CFE-19B8F436B903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>PRODUCT : ajout au cart de la sélection</t>
   </si>
   <si>
-    <t>ok - on a fait le choix d'ajouter à la quant ité existante si l'article existe déjà dans le cart</t>
-  </si>
-  <si>
     <t>affichage du cart mis à jour dans la console (affichage du local storage)</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>affichage dans la console des infos envoyées à l'API (body) - vérifier que la liste des id products est correcte après suppression d'un article du cart</t>
+  </si>
+  <si>
+    <t>ok - on a fait le choix d'écraser la quantité existante si l'article existe déjà dans le cart</t>
   </si>
 </sst>
 </file>
@@ -522,9 +522,9 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -681,10 +681,10 @@
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="44.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -692,13 +692,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>10</v>
@@ -709,13 +709,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>10</v>
@@ -726,13 +726,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>10</v>
@@ -743,13 +743,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>10</v>
@@ -760,13 +760,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>10</v>
@@ -777,13 +777,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -794,13 +794,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>10</v>
@@ -811,13 +811,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -828,13 +828,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
@@ -845,13 +845,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -862,13 +862,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>10</v>
@@ -879,13 +879,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>10</v>
@@ -896,13 +896,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>10</v>
@@ -913,13 +913,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>10</v>
@@ -930,13 +930,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>10</v>
@@ -947,13 +947,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>10</v>
@@ -964,13 +964,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>10</v>
@@ -981,13 +981,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>10</v>
@@ -998,13 +998,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
modifs commentaire plan de test
modifs commentaire plan de test
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js859\Desktop\OC\P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0DB23-1A01-4014-9CFE-19B8F436B903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90698A21-0250-47AE-8F48-B0DFAA5E6958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>ok - on a fait le choix d'écraser la quantité existante si l'article existe déjà dans le cart</t>
+  </si>
+  <si>
+    <t>affichage du cart mis à jour dans la console (affichage du local storage). Mettre en commentaire le lancement de la page suivante pour pouvoir voir la console.</t>
   </si>
 </sst>
 </file>
@@ -522,9 +525,9 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -670,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="87.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="109.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -681,7 +684,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>65</v>

</xml_diff>